<commit_message>
Deploying to gh-pages from @ eurovibes/akkupack-ng@38e2a1322359ae9fe6df4b79fb16a2588e154047 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
+++ b/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
@@ -601,7 +601,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.2+dfsg-1</t>
+    <t>9.0.1+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1186,7 +1186,8 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="5" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
@@ -2318,7 +2319,8 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/akkupack-ng@028f8ceecd0bc490bd286d1ed3742376d1a2b018 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
+++ b/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
@@ -61,13 +61,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>C101 C102 C103 C104 C105 C106 C107 C201 C202 C203 C204 C206 C207 C210 C211 C212 C213 C214 C216 C301 C302 C303 C304 C401 C402 C403 C404</t>
+    <t>C101 C102 C103 C104 C105 C106 C201 C202 C203 C204 C206 C207 C210 C211 C212 C213 C214 C216 C301 C302 C303 C304 C401 C402 C403 C404 C501</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>3.3 nF</t>
+    <t>100 nF</t>
   </si>
   <si>
     <t/>
@@ -76,10 +76,10 @@
     <t>JLCPCB</t>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/Tdk-C3216X7R1E335KT000N/C76663 https://jlcpcb.com/partdetail/53938-CL05A105KA5NQNC/C52923 https://jlcpcb.com/partdetail/291005-CL05B104KB54PNC/C307331 https://jlcpcb.com/partdetail/Yageo-CC0805KRX7R9BB221/C107145 https://jlcpcb.com/partdetail/33914-CL05C100JB5NNNC/C32949 https://jlcpcb.com/partdetail/97651-CL10A106MA8NRNC/C96446 https://jlcpcb.com/partdetail/29074-CL21B105KBFNNNE/C28323</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
+    <t>https://jlcpcb.com/partdetail/291005-CL05B104KB54PNC/C307331 https://jlcpcb.com/partdetail/53938-CL05A105KA5NQNC/C52923 https://jlcpcb.com/partdetail/Yageo-CC0805KRX7R9BB221/C107145 https://jlcpcb.com/partdetail/33914-CL05C100JB5NNNC/C32949 https://jlcpcb.com/partdetail/97651-CL10A106MA8NRNC/C96446 https://jlcpcb.com/partdetail/29074-CL21B105KBFNNNE/C28323 https://jlcpcb.com/partdetail/Tdk-C3216X7R1E335KT000N/C76663</t>
+  </si>
+  <si>
+    <t>C_0402_1005Metric</t>
   </si>
   <si>
     <t>Unpolarized capacitor</t>
@@ -172,7 +172,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D301 D401</t>
+    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D203 D204 D205 D206 D301 D401</t>
   </si>
   <si>
     <t>LED</t>
@@ -190,156 +190,159 @@
     <t>Light emitting diode</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>J101 J102 J103 J107</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>12V OUT</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2946-236-402-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
+  </si>
+  <si>
+    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>J104 J105 J106</t>
+  </si>
+  <si>
+    <t>745-302</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>2946-745-302-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
+  </si>
+  <si>
+    <t>745-302_WAGO</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>Conn_01x07</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>609-6552-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
+  </si>
+  <si>
+    <t>PinSocket_1x07_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>J203</t>
+  </si>
+  <si>
+    <t>Conn_01x06</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>952-1809-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
+  </si>
+  <si>
+    <t>PinSocket_1x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>J204 J301 J401</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>USB serial</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
+  </si>
+  <si>
+    <t>USB_Micro-AB_Molex_47590-0001</t>
+  </si>
+  <si>
+    <t>USB mini/micro connector</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>J101 J102 J103 J108</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>12V OUT</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>2946-236-402-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
-  </si>
-  <si>
-    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>J104 J105 J106</t>
-  </si>
-  <si>
-    <t>745-302</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>2946-745-302-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
-  </si>
-  <si>
-    <t>745-302_WAGO</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>J201</t>
-  </si>
-  <si>
-    <t>Conn_01x07</t>
-  </si>
-  <si>
-    <t>DISP</t>
-  </si>
-  <si>
-    <t>609-6552-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
-  </si>
-  <si>
-    <t>PinSocket_1x07_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>J203</t>
-  </si>
-  <si>
-    <t>Conn_01x06</t>
-  </si>
-  <si>
-    <t>SPI</t>
-  </si>
-  <si>
-    <t>952-1809-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
-  </si>
-  <si>
-    <t>PinSocket_1x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>J202</t>
+    <t>J502</t>
   </si>
   <si>
     <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
-    <t>SWD</t>
+    <t>Voltage sel</t>
+  </si>
+  <si>
+    <t>PinHeader_2x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>JP201</t>
+  </si>
+  <si>
+    <t>SolderJumper_2_Open</t>
+  </si>
+  <si>
+    <t>BOOT0</t>
   </si>
   <si>
     <t>--</t>
   </si>
   <si>
-    <t>Tag-Connect_TC2030-IDC-FP_2x03_P1.27mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>J204 J301 J401</t>
-  </si>
-  <si>
-    <t>USB_OTG</t>
-  </si>
-  <si>
-    <t>USB serial</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
-  </si>
-  <si>
-    <t>USB_Micro-AB_Molex_47590-0001</t>
-  </si>
-  <si>
-    <t>USB mini/micro connector</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>JP201</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Open</t>
-  </si>
-  <si>
-    <t>BOOT0</t>
-  </si>
-  <si>
     <t>SolderJumper-2_P1.3mm_Open_Pad1.0x1.5mm</t>
   </si>
   <si>
@@ -349,7 +352,7 @@
     <t>14</t>
   </si>
   <si>
-    <t>Q101 Q103 Q201</t>
+    <t>Q101 Q201 Q501</t>
   </si>
   <si>
     <t>2N7002</t>
@@ -367,7 +370,7 @@
     <t>15</t>
   </si>
   <si>
-    <t>Q102</t>
+    <t>Q502</t>
   </si>
   <si>
     <t>BSS84</t>
@@ -379,10 +382,7 @@
     <t>-0.13A Id, -50V Vds, P-Channel MOSFET, SOT-23</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117 R118 R119 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R301 R302 R401 R402</t>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R214 R215 R216 R217 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
   </si>
   <si>
     <t>R</t>
@@ -391,7 +391,7 @@
     <t>10 kΩ</t>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/26487-0402WGF1002TCE/C25744 https://jlcpcb.com/partdetail/Isabellenhuette-VMS_R010_1_0U/C466594 https://jlcpcb.com/partdetail/VikingTech-ARG03BTC3003/C335091 https://jlcpcb.com/partdetail/Yageo-RT0603BRE0716K5L/C861693 https://jlcpcb.com/partdetail/26484-0402WGF1003TCE/C25741 https://jlcpcb.com/partdetail/302237-RC02W1653FT/C321332 https://jlcpcb.com/partdetail/25819-0402WGF1000TCE/C25076 https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702 https://jlcpcb.com/partdetail/26643-0402WGF4701TCE/C25900 https://jlcpcb.com/partdetail/18646-1206W4F220JT5E/C17958 https://jlcpcb.com/partdetail/26610-0402WGF1501TCE/C25867 https://jlcpcb.com/partdetail/23677-0603WAF200JT5E/C22950 https://jlcpcb.com/partdetail/17853-0402WGF0000TCE/C17168</t>
+    <t>https://jlcpcb.com/partdetail/26487-0402WGF1002TCE/C25744 https://jlcpcb.com/partdetail/Isabellenhuette-VMS_R010_1_0U/C466594 https://jlcpcb.com/partdetail/25819-0402WGF1000TCE/C25076 https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702 https://jlcpcb.com/partdetail/26643-0402WGF4701TCE/C25900 https://jlcpcb.com/partdetail/18646-1206W4F220JT5E/C17958 https://jlcpcb.com/partdetail/26610-0402WGF1501TCE/C25867 https://jlcpcb.com/partdetail/23677-0603WAF200JT5E/C22950 https://jlcpcb.com/partdetail/17853-0402WGF0000TCE/C17168 https://jlcpcb.com/partdetail/26484-0402WGF1003TCE/C25741 https://jlcpcb.com/partdetail/302237-RC02W1653FT/C321332 https://jlcpcb.com/partdetail/VikingTech-ARG03BTC3003/C335091 https://jlcpcb.com/partdetail/Yageo-RT0603BRE0716K5L/C861693</t>
   </si>
   <si>
     <t>R_0402_1005Metric</t>
@@ -400,19 +400,19 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>36</t>
+    <t>42</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>SW101 SW201</t>
+    <t>SW201 SW501</t>
   </si>
   <si>
     <t>SW_Push_45deg</t>
   </si>
   <si>
-    <t>LED Enable</t>
+    <t>Reset</t>
   </si>
   <si>
     <t>https://jlcpcb.com/partdetail/XkbConnection-TS_1187A_B_AB/C318884</t>
@@ -619,7 +619,7 @@
     <t>Total Components:</t>
   </si>
   <si>
-    <t>J107</t>
+    <t>J501</t>
   </si>
   <si>
     <t>LED SW</t>
@@ -1236,7 +1236,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1250,7 +1250,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1278,7 +1278,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1699,7 +1699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="45" customHeight="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
@@ -1719,13 +1719,13 @@
         <v>16</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>94</v>
@@ -1734,21 +1734,21 @@
         <v>95</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>16</v>
@@ -1757,13 +1757,13 @@
         <v>16</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>100</v>
@@ -1772,7 +1772,7 @@
         <v>101</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>16</v>
@@ -1804,10 +1804,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1815,16 +1815,16 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1839,13 +1839,13 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>31</v>
@@ -1853,16 +1853,16 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1877,13 +1877,13 @@
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>12</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="24" spans="1:12" ht="225" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>120</v>
@@ -2370,7 +2370,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2384,7 +2384,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2412,7 +2412,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/akkupack-ng@7452a76cc23d1ee315b53fd179119e871243feb1 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
+++ b/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
@@ -172,7 +172,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D203 D204 D205 D206 D301 D401</t>
+    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D301 D401</t>
   </si>
   <si>
     <t>LED</t>
@@ -190,199 +190,199 @@
     <t>Light emitting diode</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>J101 J102 J103 J107</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>12V OUT</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2946-236-402-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
+  </si>
+  <si>
+    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>J104 J105 J106</t>
+  </si>
+  <si>
+    <t>745-302</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>2946-745-302-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
+  </si>
+  <si>
+    <t>745-302_WAGO</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>Conn_01x07</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>609-6552-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
+  </si>
+  <si>
+    <t>PinSocket_1x07_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>J203</t>
+  </si>
+  <si>
+    <t>Conn_01x06</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>952-1809-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
+  </si>
+  <si>
+    <t>PinSocket_1x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>J204 J301 J401</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>USB serial</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
+  </si>
+  <si>
+    <t>USB_Micro-AB_Molex_47590-0001</t>
+  </si>
+  <si>
+    <t>USB mini/micro connector</t>
+  </si>
+  <si>
+    <t>J502</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Odd_Even</t>
+  </si>
+  <si>
+    <t>Voltage sel</t>
+  </si>
+  <si>
+    <t>PinHeader_2x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>JP201</t>
+  </si>
+  <si>
+    <t>SolderJumper_2_Open</t>
+  </si>
+  <si>
+    <t>BOOT0</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>SolderJumper-2_P1.3mm_Open_Pad1.0x1.5mm</t>
+  </si>
+  <si>
+    <t>Solder Jumper, 2-pole, open</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Q101 Q201 Q501</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/9040-2N7002/C8545</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>0.115A Id, 60V Vds, N-Channel MOSFET, SOT-23</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Q502</t>
+  </si>
+  <si>
+    <t>BSS84</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/mdd_microdiode_electronics-BSS84/C427395</t>
+  </si>
+  <si>
+    <t>-0.13A Id, -50V Vds, P-Channel MOSFET, SOT-23</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>J101 J102 J103 J107</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>12V OUT</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>2946-236-402-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
-  </si>
-  <si>
-    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>J104 J105 J106</t>
-  </si>
-  <si>
-    <t>745-302</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>2946-745-302-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
-  </si>
-  <si>
-    <t>745-302_WAGO</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>J201</t>
-  </si>
-  <si>
-    <t>Conn_01x07</t>
-  </si>
-  <si>
-    <t>DISP</t>
-  </si>
-  <si>
-    <t>609-6552-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
-  </si>
-  <si>
-    <t>PinSocket_1x07_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>J203</t>
-  </si>
-  <si>
-    <t>Conn_01x06</t>
-  </si>
-  <si>
-    <t>SPI</t>
-  </si>
-  <si>
-    <t>952-1809-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
-  </si>
-  <si>
-    <t>PinSocket_1x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>J204 J301 J401</t>
-  </si>
-  <si>
-    <t>USB_OTG</t>
-  </si>
-  <si>
-    <t>USB serial</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
-  </si>
-  <si>
-    <t>USB_Micro-AB_Molex_47590-0001</t>
-  </si>
-  <si>
-    <t>USB mini/micro connector</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>J502</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>Voltage sel</t>
-  </si>
-  <si>
-    <t>PinHeader_2x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>JP201</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Open</t>
-  </si>
-  <si>
-    <t>BOOT0</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>SolderJumper-2_P1.3mm_Open_Pad1.0x1.5mm</t>
-  </si>
-  <si>
-    <t>Solder Jumper, 2-pole, open</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Q101 Q201 Q501</t>
-  </si>
-  <si>
-    <t>2N7002</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/9040-2N7002/C8545</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
-    <t>0.115A Id, 60V Vds, N-Channel MOSFET, SOT-23</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Q502</t>
-  </si>
-  <si>
-    <t>BSS84</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/mdd_microdiode_electronics-BSS84/C427395</t>
-  </si>
-  <si>
-    <t>-0.13A Id, -50V Vds, P-Channel MOSFET, SOT-23</t>
-  </si>
-  <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R214 R215 R216 R217 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
   </si>
   <si>
     <t>R</t>
@@ -400,7 +400,7 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>42</t>
+    <t>38</t>
   </si>
   <si>
     <t>17</t>
@@ -1236,7 +1236,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1250,7 +1250,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1278,7 +1278,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1739,37 +1739,37 @@
     </row>
     <row r="20" spans="1:12" ht="45" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="9" t="s">
+      <c r="K20" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>12</v>
@@ -1777,37 +1777,37 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="K21" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1815,16 +1815,16 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>111</v>
-      </c>
       <c r="D22" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1839,13 +1839,13 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="K22" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>31</v>
@@ -1853,16 +1853,16 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1877,13 +1877,13 @@
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>12</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="24" spans="1:12" ht="225" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>120</v>
@@ -2370,7 +2370,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2384,7 +2384,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2412,7 +2412,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/akkupack-ng@1b061a5c727c383a01161b62c78250f3fd715640 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
+++ b/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
@@ -172,7 +172,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D301 D401</t>
+    <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D203 D204 D205 D206 D301 D401</t>
   </si>
   <si>
     <t>LED</t>
@@ -190,126 +190,129 @@
     <t>Light emitting diode</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>J101 J102 J103 J107</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>12V OUT</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2946-236-402-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
+  </si>
+  <si>
+    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>J104 J105 J106</t>
+  </si>
+  <si>
+    <t>745-302</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>2946-745-302-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
+  </si>
+  <si>
+    <t>745-302_WAGO</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>Conn_01x07</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>609-6552-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
+  </si>
+  <si>
+    <t>PinSocket_1x07_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>J203</t>
+  </si>
+  <si>
+    <t>Conn_01x06</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>952-1809-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
+  </si>
+  <si>
+    <t>PinSocket_1x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>J204 J301 J401</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>USB serial</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
+  </si>
+  <si>
+    <t>USB_Micro-AB_Molex_47590-0001</t>
+  </si>
+  <si>
+    <t>USB mini/micro connector</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>J101 J102 J103 J107</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>12V OUT</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>2946-236-402-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/236-402/15573417</t>
-  </si>
-  <si>
-    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>J104 J105 J106</t>
-  </si>
-  <si>
-    <t>745-302</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>2946-745-302-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/wago-corporation/745-302/15557017</t>
-  </si>
-  <si>
-    <t>745-302_WAGO</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>J201</t>
-  </si>
-  <si>
-    <t>Conn_01x07</t>
-  </si>
-  <si>
-    <t>DISP</t>
-  </si>
-  <si>
-    <t>609-6552-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/amphenol-cs-fci/76341-307LF/1523892?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRACYA2AdhnIFYQBdAgBwBcoQBldgJwCWAOwDmIAL4EwVAMwIQySOmz4ipEJQAsMSowKUt9ciALV60uafPlNzNp0g9%2BwsZPDUAnAAZ5i5bgJiSDIPaio7EA4uXkFRCQJyMDDfVEwAtWDwCKjHAEkhdhwRHD54kABaY2gFKH4AV1Ugsj0QD2Y3crbqxXrG9QgmcTdKeQEAEy5ysC8Iey4TEHYAT1YcLjQsZCGgA</t>
-  </si>
-  <si>
-    <t>PinSocket_1x07_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>J203</t>
-  </si>
-  <si>
-    <t>Conn_01x06</t>
-  </si>
-  <si>
-    <t>SPI</t>
-  </si>
-  <si>
-    <t>952-1809-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/de/products/detail/harwin-inc/M20-7820646/3727777</t>
-  </si>
-  <si>
-    <t>PinSocket_1x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>J204 J301 J401</t>
-  </si>
-  <si>
-    <t>USB_OTG</t>
-  </si>
-  <si>
-    <t>USB serial</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Molex-475900001/C136001</t>
-  </si>
-  <si>
-    <t>USB_Micro-AB_Molex_47590-0001</t>
-  </si>
-  <si>
-    <t>USB mini/micro connector</t>
-  </si>
-  <si>
     <t>J502</t>
   </si>
   <si>
@@ -379,10 +382,7 @@
     <t>-0.13A Id, -50V Vds, P-Channel MOSFET, SOT-23</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R214 R215 R216 R217 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
   </si>
   <si>
     <t>R</t>
@@ -400,7 +400,7 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>38</t>
+    <t>42</t>
   </si>
   <si>
     <t>17</t>
@@ -1236,7 +1236,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1250,7 +1250,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1278,7 +1278,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1739,16 +1739,16 @@
     </row>
     <row r="20" spans="1:12" ht="45" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>16</v>
@@ -1766,10 +1766,10 @@
         <v>16</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>12</v>
@@ -1777,16 +1777,16 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>16</v>
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>16</v>
@@ -1804,10 +1804,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1815,16 +1815,16 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1839,13 +1839,13 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>31</v>
@@ -1853,16 +1853,16 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1877,13 +1877,13 @@
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>12</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="24" spans="1:12" ht="225" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>120</v>
@@ -2370,7 +2370,7 @@
         <v>195</v>
       </c>
       <c r="F3" s="3">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2384,7 +2384,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="3">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2412,7 +2412,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="3">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/akkupack-ng@d31a38aa6fd3fc88e2c7c42599cf834df72fc93f 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
+++ b/Fabrication/BoM/akkupack-ng-bom_0.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="223">
   <si>
     <t>Row</t>
   </si>
@@ -133,6 +133,27 @@
     <t>75V 0.15A Fast switching Diode, SOD-323</t>
   </si>
   <si>
+    <t>D207 D208</t>
+  </si>
+  <si>
+    <t>D_Zener_Dual_CommonAnode_KKA</t>
+  </si>
+  <si>
+    <t>AZ23C5V6-7</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/DiodesIncorporated-AZ23C5V6_7F/C98737</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>Dual Zener diode, common anode on pin 3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>D101</t>
   </si>
   <si>
@@ -151,7 +172,7 @@
     <t>500mW Zener Diode, SOD-123F</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>D201</t>
@@ -169,7 +190,7 @@
     <t>ESD protection diode, 3.3Vrwm, SOD-923</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D203 D204 D205 D206 D301 D401</t>
@@ -193,7 +214,7 @@
     <t>16</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>J101 J102 J103 J107</t>
@@ -220,7 +241,7 @@
     <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>J104 J105 J106</t>
@@ -241,7 +262,7 @@
     <t>745-302_WAGO</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>J201</t>
@@ -265,7 +286,7 @@
     <t>Generic connector, single row, 01x07, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>J203</t>
@@ -289,7 +310,7 @@
     <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>J204 J301 J401</t>
@@ -310,7 +331,7 @@
     <t>USB mini/micro connector</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>J502</t>
@@ -322,13 +343,19 @@
     <t>Voltage sel</t>
   </si>
   <si>
+    <t>TME</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/details/zl202-6g/stiftleisten-und-buchsen/connfly/ds1021-2-3sf11-b/</t>
+  </si>
+  <si>
     <t>PinHeader_2x03_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>JP201</t>
@@ -349,7 +376,7 @@
     <t>Solder Jumper, 2-pole, open</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Q101 Q201 Q501</t>
@@ -361,15 +388,9 @@
     <t>https://jlcpcb.com/partdetail/9040-2N7002/C8545</t>
   </si>
   <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>0.115A Id, 60V Vds, N-Channel MOSFET, SOT-23</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Q502</t>
   </si>
   <si>
@@ -382,7 +403,10 @@
     <t>-0.13A Id, -50V Vds, P-Channel MOSFET, SOT-23</t>
   </si>
   <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R214 R215 R216 R217 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
+    <t>17</t>
+  </si>
+  <si>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R201 R202 R203 R204 R205 R206 R207 R208 R209 R210 R211 R212 R213 R214 R215 R216 R217 R218 R219 R220 R221 R301 R302 R401 R402 R501 R502 R503 R504 R505 R506 R507</t>
   </si>
   <si>
     <t>R</t>
@@ -400,10 +424,10 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>46</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>SW201 SW501</t>
@@ -424,7 +448,7 @@
     <t>Push button switch, normally open, two pins, 45° tilted</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>U102 U103</t>
@@ -442,7 +466,7 @@
     <t>8-bit serial-in parallel-out shift register</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>U203</t>
@@ -460,7 +484,7 @@
     <t>1A Low Dropout regulator, positive, 3.3V fixed output, SOT-223</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>U101</t>
@@ -475,7 +499,7 @@
     <t>SOP65P640X120-14N</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>U303 U403</t>
@@ -493,7 +517,7 @@
     <t>USB serial converter, UART, SOIC-8</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>U201</t>
@@ -514,7 +538,7 @@
     <t>STMicroelectronics Arm Cortex-M3 MCU, 128KB flash, 20KB RAM, 72 MHz, 2.0-3.6V, 37 GPIO, LQFP48</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>U202 U301 U401</t>
@@ -532,7 +556,7 @@
     <t>Very low capacitance ESD protection diode, 2 data-line, SOT-23-6</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>U302 U402</t>
@@ -550,7 +574,7 @@
     <t>Positive 60-250mA Low Dropout Regulator, Fixed Output, SOT-23</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Y201 Y202</t>
@@ -617,6 +641,27 @@
   </si>
   <si>
     <t>Total Components:</t>
+  </si>
+  <si>
+    <t>J205</t>
+  </si>
+  <si>
+    <t>Conn_01x04</t>
+  </si>
+  <si>
+    <t>EXT I2C</t>
+  </si>
+  <si>
+    <t>WM4113-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/de/products/detail/molex/0022272041/1130579</t>
+  </si>
+  <si>
+    <t>Molex_KK-254_AE-6410-04A_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x04, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
     <t>J501</t>
@@ -796,8 +841,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1018254</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:colOff>418179</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>58841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -847,9 +892,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>456279</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>465804</xdr:colOff>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>58841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1174,7 +1219,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1185,7 +1230,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
@@ -1199,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1213,55 +1258,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F2" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="F3" s="3">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="F4" s="3">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1269,16 +1314,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F6" s="3">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1433,7 +1478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>30</v>
       </c>
@@ -1468,7 +1513,7 @@
         <v>42</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1482,7 +1527,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
@@ -1497,27 +1542,27 @@
         <v>16</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="60" customHeight="1">
+    <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>52</v>
@@ -1544,86 +1589,86 @@
         <v>55</v>
       </c>
       <c r="L14" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="K15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="L15" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="E16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="H16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="10" t="s">
+      <c r="I16" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="L16" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="105" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
@@ -1643,7 +1688,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>77</v>
@@ -1655,74 +1700,74 @@
         <v>79</v>
       </c>
       <c r="K17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="105" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="K18" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>93</v>
@@ -1734,10 +1779,10 @@
         <v>95</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="8" t="s">
         <v>96</v>
       </c>
@@ -1757,36 +1802,36 @@
         <v>16</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>16</v>
@@ -1795,19 +1840,19 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1815,16 +1860,16 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1833,36 +1878,36 @@
         <v>16</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="30" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1877,30 +1922,30 @@
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="225" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>16</v>
@@ -1915,19 +1960,19 @@
         <v>16</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="225" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -1962,21 +2007,21 @@
         <v>133</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>16</v>
@@ -1991,13 +2036,13 @@
         <v>16</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>22</v>
@@ -2005,16 +2050,16 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>16</v>
@@ -2029,30 +2074,30 @@
         <v>16</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>16</v>
@@ -2067,13 +2112,13 @@
         <v>16</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>12</v>
@@ -2081,16 +2126,16 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>16</v>
@@ -2105,30 +2150,30 @@
         <v>16</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>156</v>
+        <v>16</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>16</v>
@@ -2143,30 +2188,30 @@
         <v>16</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>16</v>
@@ -2181,30 +2226,30 @@
         <v>16</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>16</v>
@@ -2219,30 +2264,30 @@
         <v>16</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="45" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>16</v>
@@ -2257,15 +2302,53 @@
         <v>16</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L33" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="45" customHeight="1">
+      <c r="A34" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2299,16 +2382,17 @@
     <hyperlink ref="H31" r:id="rId23"/>
     <hyperlink ref="H32" r:id="rId24"/>
     <hyperlink ref="H33" r:id="rId25"/>
+    <hyperlink ref="H34" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId27"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2326,14 +2410,14 @@
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="42.7109375" customWidth="1"/>
+    <col min="10" max="10" width="51.7109375" customWidth="1"/>
     <col min="11" max="11" width="60.7109375" customWidth="1"/>
     <col min="12" max="12" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2347,55 +2431,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F2" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="F3" s="3">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="F4" s="3">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2403,16 +2487,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F6" s="3">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2458,13 +2542,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>208</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>16</v>
@@ -2473,21 +2557,59 @@
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>65</v>
+        <v>213</v>
       </c>
       <c r="L9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2497,10 +2619,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1"/>
+    <hyperlink ref="H10" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2517,22 +2640,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>